<commit_message>
Updated index data - numbers & increased sd
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230927.xlsx
+++ b/data/hake_intrasp_230927.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4301AEE4-FADF-6F4B-AD91-C2C7C34274B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF1DB98-A3E8-754C-B16E-0F825FB9B0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1587,7 +1587,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16724,7 +16724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P2" sqref="P2:U2"/>
     </sheetView>
   </sheetViews>
@@ -16870,7 +16870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:V2"/>
     </sheetView>
   </sheetViews>
@@ -17022,7 +17022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:V2"/>
     </sheetView>
   </sheetViews>
@@ -21601,8 +21601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24727,7 +24727,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24938,7 +24938,7 @@
         <v>20</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -24984,7 +24984,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25049,7 +25049,7 @@
         <v>1318035</v>
       </c>
       <c r="I2">
-        <v>8.5900000000000004E-2</v>
+        <v>0.33478599999999997</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -25136,7 +25136,7 @@
         <v>1569148</v>
       </c>
       <c r="I5">
-        <v>4.5999999999999999E-2</v>
+        <v>0.29488599999999998</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -25223,7 +25223,7 @@
         <v>861744</v>
       </c>
       <c r="I8">
-        <v>0.10199999999999999</v>
+        <v>0.35088599999999998</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -25281,7 +25281,7 @@
         <v>2137528</v>
       </c>
       <c r="I10">
-        <v>6.1899999999999997E-2</v>
+        <v>0.31078600000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -25339,7 +25339,7 @@
         <v>1376099</v>
       </c>
       <c r="I12">
-        <v>6.1600000000000002E-2</v>
+        <v>0.31048599999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -25397,7 +25397,7 @@
         <v>942721</v>
       </c>
       <c r="I14">
-        <v>7.3800000000000004E-2</v>
+        <v>0.32268599999999997</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -25455,7 +25455,7 @@
         <v>1502273</v>
       </c>
       <c r="I16">
-        <v>9.5699999999999993E-2</v>
+        <v>0.344586</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -25513,7 +25513,7 @@
         <v>674617</v>
       </c>
       <c r="I18">
-        <v>0.1133</v>
+        <v>0.36218600000000001</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -25542,7 +25542,7 @@
         <v>1279421</v>
       </c>
       <c r="I19">
-        <v>6.4699999999999994E-2</v>
+        <v>0.31358599999999998</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -25571,7 +25571,7 @@
         <v>1929235</v>
       </c>
       <c r="I20">
-        <v>6.2E-2</v>
+        <v>0.310886</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -25629,7 +25629,7 @@
         <v>2155853</v>
       </c>
       <c r="I22">
-        <v>8.09E-2</v>
+        <v>0.32978600000000002</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -25687,7 +25687,7 @@
         <v>1417811</v>
       </c>
       <c r="I24">
-        <v>6.3200000000000006E-2</v>
+        <v>0.31208599999999997</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -25745,7 +25745,7 @@
         <v>1722611</v>
       </c>
       <c r="I26">
-        <v>6.1899999999999997E-2</v>
+        <v>0.31078600000000001</v>
       </c>
     </row>
   </sheetData>
@@ -27206,7 +27206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:DU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Small update to proportion mature in data file
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230927.xlsx
+++ b/data/hake_intrasp_230927.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF1DB98-A3E8-754C-B16E-0F825FB9B0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BE3025-3AA5-DD4F-A992-3845D8D2A09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="20500" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1586,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="D16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -16578,8 +16578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21601,7 +21601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>

</xml_diff>